<commit_message>
Wir haben viele Probleme
</commit_message>
<xml_diff>
--- a/2. Doble-Slit/TRABAJO EN CLASE/TRABAJO EN CLASE.xlsx
+++ b/2. Doble-Slit/TRABAJO EN CLASE/TRABAJO EN CLASE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0bb2241ed02e8b1/Desktop/GITHUB/Lab-Intermedio/2. Doble-Slit/TRABAJO EN CLASE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juank\Escritorio\Universidad\202420\Lab Intemedio\Lab-Intermedio\2. Doble-Slit\TRABAJO EN CLASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="318" documentId="11_AD4D2F04E46CFB4ACB3E20FAA5D6EA76683EDF2F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F992E972-CEFB-4907-A67D-F0715252E954}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3B2224-C408-4801-8E1B-F64B89BC5D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,9 +144,10 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -156,10 +157,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4190,21 +4190,21 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
@@ -4248,25 +4248,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A25AFD-A5B0-4D4F-9012-CF20E08D366E}">
   <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4367,7 +4367,7 @@
       <c r="F6">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="O6" s="8"/>
+      <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -4628,7 +4628,7 @@
       <c r="F19">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="P19" s="8"/>
+      <c r="P19" s="4"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -4689,7 +4689,7 @@
       <c r="F22">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="Q22" s="8"/>
+      <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -5324,9 +5324,6 @@
       <c r="D54">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E54">
-        <v>9.0999999999999801</v>
-      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -5341,9 +5338,6 @@
       <c r="D55">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E55">
-        <v>9.1999999999999797</v>
-      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -5358,9 +5352,6 @@
       <c r="D56">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E56">
-        <v>9.2999999999999794</v>
-      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -5375,9 +5366,6 @@
       <c r="D57">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E57">
-        <v>9.3999999999999808</v>
-      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
@@ -5392,9 +5380,6 @@
       <c r="D58">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E58">
-        <v>9.4999999999999805</v>
-      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
@@ -5572,7 +5557,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>7.8</v>
       </c>
@@ -5580,7 +5565,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>7.9</v>
       </c>
@@ -5588,7 +5573,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>8</v>
       </c>
@@ -5596,7 +5581,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>8.1</v>
       </c>
@@ -5604,7 +5589,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>8.1999999999999993</v>
       </c>
@@ -5612,7 +5597,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>8.3000000000000007</v>
       </c>
@@ -5620,7 +5605,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>8.4</v>
       </c>
@@ -5628,7 +5613,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>8.5</v>
       </c>
@@ -5636,433 +5621,316 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>8.6</v>
       </c>
       <c r="B89">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="C89">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>8.6999999999999993</v>
       </c>
       <c r="B90">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="C90">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>8.8000000000000007</v>
       </c>
       <c r="B91">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="C91">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>8.9</v>
       </c>
       <c r="B92">
         <v>0.05</v>
       </c>
-      <c r="C92">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>9</v>
       </c>
       <c r="B93">
         <v>2.4E-2</v>
       </c>
-      <c r="C93">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>9.1</v>
       </c>
       <c r="B94">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="C94">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>9.1999999999999993</v>
       </c>
       <c r="B95">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="C95">
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>9.3000000000000007</v>
       </c>
       <c r="B96">
         <v>0.04</v>
       </c>
-      <c r="C96">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>9.4</v>
       </c>
       <c r="B97">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="C97">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>9.5</v>
       </c>
       <c r="B98">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="C98">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>9.6</v>
       </c>
       <c r="B99">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="C99">
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>9.6999999999999993</v>
       </c>
       <c r="B100">
         <v>2.3E-2</v>
       </c>
-      <c r="C100">
-        <v>9.6999999999999993</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>9.8000000000000007</v>
       </c>
       <c r="B101">
         <v>1.2E-2</v>
       </c>
-      <c r="C101">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>9.9</v>
       </c>
       <c r="B102">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="C102">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>10</v>
       </c>
       <c r="B103">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="C103">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>10.1</v>
       </c>
       <c r="B104">
         <v>0.01</v>
       </c>
-      <c r="C104">
-        <v>10.1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>10.199999999999999</v>
       </c>
       <c r="B105">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C105">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>10.3</v>
       </c>
       <c r="B106">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C106">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>10.4</v>
       </c>
       <c r="B107">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C107">
-        <v>10.4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>10.5</v>
       </c>
       <c r="B108">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C108">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>10.6</v>
       </c>
       <c r="B109">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="C109">
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>10.7</v>
       </c>
       <c r="B110">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C110">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>10.8</v>
       </c>
       <c r="B111">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="C111">
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>10.9</v>
       </c>
       <c r="B112">
         <v>1.9E-2</v>
       </c>
-      <c r="C112">
-        <v>10.9</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>11</v>
       </c>
       <c r="B113">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C113">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>11.1</v>
       </c>
       <c r="B114">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C114">
-        <v>11.1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>11.2</v>
       </c>
       <c r="B115">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="C115">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>11.3</v>
       </c>
       <c r="B116">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="C116">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>11.4</v>
       </c>
       <c r="B117">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="C117">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>11.5</v>
       </c>
       <c r="B118">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="C118">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>11.6</v>
       </c>
       <c r="B119">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C119">
-        <v>11.6</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>11.7</v>
       </c>
       <c r="B120">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="C120">
-        <v>11.7</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>11.8</v>
       </c>
       <c r="B121">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="C121">
-        <v>11.8</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>11.9</v>
       </c>
       <c r="B122">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="C122">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>12</v>
       </c>
       <c r="B123">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="C123">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>12.1</v>
       </c>
       <c r="B124">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="C124">
-        <v>12.1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>12.2</v>
       </c>
       <c r="B125">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="C125">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>12.3</v>
       </c>
       <c r="B126">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="C126">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>12.4</v>
       </c>
       <c r="B127">
         <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="C127">
-        <v>12.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>